<commit_message>
a few bugs solved in player standings
</commit_message>
<xml_diff>
--- a/Backup/tournament/player_standings.xlsx
+++ b/Backup/tournament/player_standings.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IIT\1st Year\1st Trimester\CM1601 [PRO]  Programming Fundamentals\Course Work\tournament\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8416D071-82ED-4AAC-98D8-28DA286B6D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="6810" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -298,8 +292,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,14 +356,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -416,7 +402,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -448,27 +434,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,24 +468,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -693,16 +643,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -713,972 +661,972 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>258</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>197</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>186</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>284</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>156</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>151</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>23</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>27</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" t="s">
         <v>32</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="C31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>33</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33" t="s">
         <v>34</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
       <c r="A34" t="s">
         <v>35</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="C34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>36</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3">
       <c r="A36" t="s">
         <v>37</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>229</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>38</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="C41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42" t="s">
         <v>43</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>171</v>
       </c>
       <c r="C42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>44</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="C43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44" t="s">
         <v>45</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="C44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
       <c r="A45" t="s">
         <v>46</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="C45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>47</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>174</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3">
       <c r="A47" t="s">
         <v>48</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="C47">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>49</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="C48">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3">
       <c r="A49" t="s">
         <v>50</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C49">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3">
       <c r="A50" t="s">
         <v>51</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="C50">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>52</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="C51">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3">
       <c r="A52" t="s">
         <v>53</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C52">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>54</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="C53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>55</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>159</v>
       </c>
       <c r="C54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>56</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="C55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>57</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="C56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>58</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>181</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>59</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>179</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3">
       <c r="A59" t="s">
         <v>60</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>221</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3">
       <c r="A60" t="s">
         <v>61</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3">
       <c r="A61" t="s">
         <v>62</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3">
       <c r="A62" t="s">
         <v>63</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3">
       <c r="A63" t="s">
         <v>64</v>
       </c>
       <c r="B63">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="C63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
       <c r="A64" t="s">
         <v>65</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="C64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
       <c r="A65" t="s">
         <v>66</v>
       </c>
       <c r="B65">
-        <v>0</v>
+        <v>111</v>
       </c>
       <c r="C65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
       <c r="A66" t="s">
         <v>67</v>
       </c>
       <c r="B66">
-        <v>0</v>
+        <v>112</v>
       </c>
       <c r="C66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
       <c r="A67" t="s">
         <v>68</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>107</v>
       </c>
       <c r="C67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
       <c r="A68" t="s">
         <v>69</v>
       </c>
       <c r="B68">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="C68">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3">
       <c r="A69" t="s">
         <v>70</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="C69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3">
       <c r="A70" t="s">
         <v>71</v>
       </c>
       <c r="B70">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="C70">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3">
       <c r="A71" t="s">
         <v>72</v>
       </c>
       <c r="B71">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3">
       <c r="A72" t="s">
         <v>73</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3">
       <c r="A73" t="s">
         <v>74</v>
       </c>
       <c r="B73">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C73">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3">
       <c r="A74" t="s">
         <v>75</v>
       </c>
       <c r="B74">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="C74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
       <c r="A75" t="s">
         <v>76</v>
       </c>
       <c r="B75">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="C75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
       <c r="A76" t="s">
         <v>77</v>
       </c>
       <c r="B76">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
       <c r="A77" t="s">
         <v>78</v>
       </c>
       <c r="B77">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
       <c r="A78" t="s">
         <v>79</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
       <c r="A79" t="s">
         <v>80</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>163</v>
       </c>
       <c r="C79">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3">
       <c r="A80" t="s">
         <v>81</v>
       </c>
       <c r="B80">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" t="s">
         <v>82</v>
       </c>
       <c r="B81">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" t="s">
         <v>83</v>
       </c>
       <c r="B82">
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" t="s">
         <v>84</v>
       </c>
       <c r="B83">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" t="s">
         <v>85</v>
       </c>
       <c r="B84">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="C84">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" t="s">
         <v>86</v>
       </c>
       <c r="B85">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="C85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
       <c r="A86" t="s">
         <v>87</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
       <c r="A87" t="s">
         <v>88</v>
       </c>
       <c r="B87">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="C87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
       <c r="A88" t="s">
         <v>89</v>
       </c>
       <c r="B88">
-        <v>0</v>
+        <v>174</v>
       </c>
       <c r="C88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
       <c r="A89" t="s">
         <v>90</v>
       </c>
       <c r="B89">
-        <v>0</v>
+        <v>89</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>